<commit_message>
updated legacy GSC data files
</commit_message>
<xml_diff>
--- a/gsc-export-old/Coverage.xlsx
+++ b/gsc-export-old/Coverage.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -29,13 +29,10 @@
     <t>Impressions</t>
   </si>
   <si>
-    <t>2025-08-19</t>
+    <t>2025-08-20</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>2025-08-20</t>
   </si>
   <si>
     <t>2025-08-21</t>
@@ -397,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -428,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -456,21 +453,21 @@
         <v>5</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>5</v>
+      <c r="B5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>8.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
@@ -484,7 +481,7 @@
         <v>8.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +495,7 @@
         <v>8.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +509,7 @@
         <v>8.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
@@ -520,10 +517,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>8.0</v>
+        <v>20.0</v>
       </c>
       <c r="D9" t="n" s="0">
         <v>6.0</v>
@@ -540,7 +537,7 @@
         <v>20.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -554,7 +551,7 @@
         <v>20.0</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +565,7 @@
         <v>20.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -576,13 +573,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>20.0</v>
+        <v>23.0</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
@@ -596,7 +593,7 @@
         <v>23.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="15">
@@ -610,7 +607,7 @@
         <v>23.0</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="16">
@@ -624,7 +621,7 @@
         <v>23.0</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="17">
@@ -638,7 +635,7 @@
         <v>23.0</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -652,7 +649,7 @@
         <v>23.0</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="19">
@@ -680,7 +677,7 @@
         <v>23.0</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="21">
@@ -694,7 +691,7 @@
         <v>23.0</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="22">
@@ -708,7 +705,7 @@
         <v>23.0</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">
@@ -716,13 +713,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="n" s="0">
-        <v>4.0</v>
+        <v>11.0</v>
       </c>
       <c r="C23" t="n" s="0">
-        <v>23.0</v>
+        <v>38.0</v>
       </c>
       <c r="D23" t="n" s="0">
-        <v>5.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="24">
@@ -736,7 +733,7 @@
         <v>38.0</v>
       </c>
       <c r="D24" t="n" s="0">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="25">
@@ -750,7 +747,7 @@
         <v>38.0</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>19.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="26">
@@ -764,7 +761,7 @@
         <v>38.0</v>
       </c>
       <c r="D26" t="n" s="0">
-        <v>11.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="27">
@@ -772,13 +769,13 @@
         <v>30</v>
       </c>
       <c r="B27" t="n" s="0">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="C27" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
         <v>38.0</v>
-      </c>
-      <c r="D27" t="n" s="0">
-        <v>18.0</v>
       </c>
     </row>
     <row r="28">
@@ -792,7 +789,7 @@
         <v>45.0</v>
       </c>
       <c r="D28" t="n" s="0">
-        <v>38.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +803,7 @@
         <v>45.0</v>
       </c>
       <c r="D29" t="n" s="0">
-        <v>46.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="30">
@@ -817,10 +814,10 @@
         <v>4.0</v>
       </c>
       <c r="C30" t="n" s="0">
-        <v>45.0</v>
+        <v>55.0</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>35.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="31">
@@ -834,7 +831,7 @@
         <v>55.0</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>23.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="32">
@@ -848,7 +845,7 @@
         <v>55.0</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>33.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="33">
@@ -862,7 +859,7 @@
         <v>55.0</v>
       </c>
       <c r="D33" t="n" s="0">
-        <v>41.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="34">
@@ -870,13 +867,13 @@
         <v>37</v>
       </c>
       <c r="B34" t="n" s="0">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="C34" t="n" s="0">
-        <v>55.0</v>
+        <v>60.0</v>
       </c>
       <c r="D34" t="n" s="0">
-        <v>46.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="35">
@@ -890,7 +887,7 @@
         <v>60.0</v>
       </c>
       <c r="D35" t="n" s="0">
-        <v>44.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="36">
@@ -904,7 +901,7 @@
         <v>60.0</v>
       </c>
       <c r="D36" t="n" s="0">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="37">
@@ -912,13 +909,13 @@
         <v>40</v>
       </c>
       <c r="B37" t="n" s="0">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" t="n" s="0">
-        <v>60.0</v>
+        <v>76.0</v>
       </c>
       <c r="D37" t="n" s="0">
-        <v>35.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="38">
@@ -932,7 +929,7 @@
         <v>76.0</v>
       </c>
       <c r="D38" t="n" s="0">
-        <v>38.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="39">
@@ -946,7 +943,7 @@
         <v>76.0</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>42.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="40">
@@ -960,7 +957,7 @@
         <v>76.0</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>40.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="41">
@@ -968,13 +965,13 @@
         <v>44</v>
       </c>
       <c r="B41" t="n" s="0">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="C41" t="n" s="0">
-        <v>76.0</v>
+        <v>88.0</v>
       </c>
       <c r="D41" t="n" s="0">
-        <v>43.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="42">
@@ -988,7 +985,7 @@
         <v>88.0</v>
       </c>
       <c r="D42" t="n" s="0">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="43">
@@ -1002,7 +999,7 @@
         <v>88.0</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>41.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="44">
@@ -1010,13 +1007,13 @@
         <v>47</v>
       </c>
       <c r="B44" t="n" s="0">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="C44" t="n" s="0">
-        <v>88.0</v>
+        <v>119.0</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>30.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="45">
@@ -1030,7 +1027,7 @@
         <v>119.0</v>
       </c>
       <c r="D45" t="n" s="0">
-        <v>52.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="46">
@@ -1044,7 +1041,7 @@
         <v>119.0</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>61.0</v>
+        <v>87.0</v>
       </c>
     </row>
     <row r="47">
@@ -1058,7 +1055,7 @@
         <v>119.0</v>
       </c>
       <c r="D47" t="n" s="0">
-        <v>87.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="48">
@@ -1066,13 +1063,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="n" s="0">
-        <v>8.0</v>
+        <v>147.0</v>
       </c>
       <c r="C48" t="n" s="0">
-        <v>119.0</v>
+        <v>130.0</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>104.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="49">
@@ -1086,7 +1083,7 @@
         <v>130.0</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>77.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="50">
@@ -1100,7 +1097,7 @@
         <v>130.0</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>67.0</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="51">
@@ -1108,13 +1105,13 @@
         <v>54</v>
       </c>
       <c r="B51" t="n" s="0">
-        <v>147.0</v>
+        <v>4.0</v>
       </c>
       <c r="C51" t="n" s="0">
         <v>130.0</v>
       </c>
       <c r="D51" t="n" s="0">
-        <v>83.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="52">
@@ -1128,7 +1125,7 @@
         <v>130.0</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>67.0</v>
+        <v>85.0</v>
       </c>
     </row>
     <row r="53">
@@ -1142,7 +1139,7 @@
         <v>130.0</v>
       </c>
       <c r="D53" t="n" s="0">
-        <v>85.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="54">
@@ -1156,7 +1153,7 @@
         <v>130.0</v>
       </c>
       <c r="D54" t="n" s="0">
-        <v>48.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="55">
@@ -1164,13 +1161,13 @@
         <v>58</v>
       </c>
       <c r="B55" t="n" s="0">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C55" t="n" s="0">
-        <v>130.0</v>
+        <v>128.0</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>52.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="56">
@@ -1184,7 +1181,7 @@
         <v>128.0</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>61.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="57">
@@ -1198,7 +1195,7 @@
         <v>128.0</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>54.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="58">
@@ -1206,13 +1203,13 @@
         <v>61</v>
       </c>
       <c r="B58" t="n" s="0">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C58" t="n" s="0">
-        <v>128.0</v>
+        <v>127.0</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>45.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="59">
@@ -1226,7 +1223,7 @@
         <v>127.0</v>
       </c>
       <c r="D59" t="n" s="0">
-        <v>46.0</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="60">
@@ -1240,7 +1237,7 @@
         <v>127.0</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>74.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="61">
@@ -1254,7 +1251,7 @@
         <v>127.0</v>
       </c>
       <c r="D61" t="n" s="0">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="62">
@@ -1262,13 +1259,13 @@
         <v>65</v>
       </c>
       <c r="B62" t="n" s="0">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C62" t="n" s="0">
-        <v>127.0</v>
+        <v>126.0</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>61.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="63">
@@ -1282,7 +1279,7 @@
         <v>126.0</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>54.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="64">
@@ -1296,7 +1293,7 @@
         <v>126.0</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>51.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="65">
@@ -1304,13 +1301,13 @@
         <v>68</v>
       </c>
       <c r="B65" t="n" s="0">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
       <c r="C65" t="n" s="0">
-        <v>126.0</v>
+        <v>121.0</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>36.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="66">
@@ -1324,7 +1321,7 @@
         <v>121.0</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>55.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="67">
@@ -1338,7 +1335,7 @@
         <v>121.0</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>41.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="68">
@@ -1352,7 +1349,7 @@
         <v>121.0</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>56.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="69">
@@ -1360,13 +1357,13 @@
         <v>72</v>
       </c>
       <c r="B69" t="n" s="0">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="C69" t="n" s="0">
-        <v>121.0</v>
+        <v>115.0</v>
       </c>
       <c r="D69" t="n" s="0">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="70">
@@ -1380,7 +1377,7 @@
         <v>115.0</v>
       </c>
       <c r="D70" t="n" s="0">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="71">
@@ -1394,7 +1391,7 @@
         <v>115.0</v>
       </c>
       <c r="D71" t="n" s="0">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="72">
@@ -1402,13 +1399,13 @@
         <v>75</v>
       </c>
       <c r="B72" t="n" s="0">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C72" t="n" s="0">
-        <v>115.0</v>
+        <v>114.0</v>
       </c>
       <c r="D72" t="n" s="0">
-        <v>23.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="73">
@@ -1422,7 +1419,7 @@
         <v>114.0</v>
       </c>
       <c r="D73" t="n" s="0">
-        <v>28.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="74">
@@ -1436,7 +1433,7 @@
         <v>114.0</v>
       </c>
       <c r="D74" t="n" s="0">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="75">
@@ -1450,7 +1447,7 @@
         <v>114.0</v>
       </c>
       <c r="D75" t="n" s="0">
-        <v>30.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="76">
@@ -1458,13 +1455,13 @@
         <v>79</v>
       </c>
       <c r="B76" t="n" s="0">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
       <c r="C76" t="n" s="0">
-        <v>114.0</v>
+        <v>107.0</v>
       </c>
       <c r="D76" t="n" s="0">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="77">
@@ -1478,7 +1475,7 @@
         <v>107.0</v>
       </c>
       <c r="D77" t="n" s="0">
-        <v>25.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="78">
@@ -1492,7 +1489,7 @@
         <v>107.0</v>
       </c>
       <c r="D78" t="n" s="0">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="79">
@@ -1500,13 +1497,13 @@
         <v>82</v>
       </c>
       <c r="B79" t="n" s="0">
-        <v>28.0</v>
+        <v>36.0</v>
       </c>
       <c r="C79" t="n" s="0">
-        <v>107.0</v>
+        <v>99.0</v>
       </c>
       <c r="D79" t="n" s="0">
-        <v>28.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="80">
@@ -1520,7 +1517,7 @@
         <v>99.0</v>
       </c>
       <c r="D80" t="n" s="0">
-        <v>13.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="81">
@@ -1534,7 +1531,7 @@
         <v>99.0</v>
       </c>
       <c r="D81" t="n" s="0">
-        <v>19.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="82">
@@ -1548,7 +1545,7 @@
         <v>99.0</v>
       </c>
       <c r="D82" t="n" s="0">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="83">
@@ -1562,7 +1559,7 @@
         <v>99.0</v>
       </c>
       <c r="D83" t="n" s="0">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="84">
@@ -1576,7 +1573,7 @@
         <v>99.0</v>
       </c>
       <c r="D84" t="n" s="0">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="85">
@@ -1590,20 +1587,6 @@
         <v>99.0</v>
       </c>
       <c r="D85" t="n" s="0">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="B86" t="n" s="0">
-        <v>36.0</v>
-      </c>
-      <c r="C86" t="n" s="0">
-        <v>99.0</v>
-      </c>
-      <c r="D86" t="n" s="0">
         <v>9.0</v>
       </c>
     </row>
@@ -1622,27 +1605,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s" s="0">
         <v>92</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>93</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>95</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>96</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
@@ -1650,13 +1633,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>97</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>98</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>22.0</v>
@@ -1664,13 +1647,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>1.0</v>
@@ -1678,13 +1661,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>100</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>101</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>0.0</v>
@@ -1692,13 +1675,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>103</v>
-      </c>
       <c r="C6" t="s" s="0">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>6.0</v>
@@ -1706,13 +1689,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>4.0</v>
@@ -1720,13 +1703,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>105</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>106</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>0.0</v>
@@ -1747,16 +1730,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s" s="0">
         <v>92</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1774,18 +1757,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>107</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>109</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated legacy GSC export data
</commit_message>
<xml_diff>
--- a/gsc-export-old/Coverage.xlsx
+++ b/gsc-export-old/Coverage.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>2025-11-11</t>
+  </si>
+  <si>
+    <t>2025-11-12</t>
+  </si>
+  <si>
+    <t>2025-11-13</t>
+  </si>
+  <si>
+    <t>2025-11-14</t>
+  </si>
+  <si>
+    <t>2025-11-15</t>
   </si>
   <si>
     <t>Reason</t>
@@ -394,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -1588,6 +1600,62 @@
       </c>
       <c r="D85" t="n" s="0">
         <v>9.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B86" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="C86" t="n" s="0">
+        <v>97.0</v>
+      </c>
+      <c r="D86" t="n" s="0">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B87" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="C87" t="n" s="0">
+        <v>97.0</v>
+      </c>
+      <c r="D87" t="n" s="0">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B88" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="C88" t="n" s="0">
+        <v>97.0</v>
+      </c>
+      <c r="D88" t="n" s="0">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B89" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="C89" t="n" s="0">
+        <v>97.0</v>
+      </c>
+      <c r="D89" t="n" s="0">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>
@@ -1605,27 +1673,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
@@ -1633,27 +1701,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>94</v>
-      </c>
       <c r="C4" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>1.0</v>
@@ -1661,13 +1729,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>0.0</v>
@@ -1675,13 +1743,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>6.0</v>
@@ -1689,13 +1757,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>4.0</v>
@@ -1703,13 +1771,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>0.0</v>
@@ -1730,16 +1798,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1757,18 +1825,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated legacy GSC export files
</commit_message>
<xml_diff>
--- a/gsc-export-old/Coverage.xlsx
+++ b/gsc-export-old/Coverage.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -29,18 +29,12 @@
     <t>Impressions</t>
   </si>
   <si>
-    <t>2025-09-01</t>
+    <t>2025-09-03</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2025-09-02</t>
-  </si>
-  <si>
-    <t>2025-09-03</t>
-  </si>
-  <si>
     <t>2025-09-04</t>
   </si>
   <si>
@@ -269,6 +263,18 @@
     <t>2025-11-18</t>
   </si>
   <si>
+    <t>2025-11-19</t>
+  </si>
+  <si>
+    <t>2025-11-20</t>
+  </si>
+  <si>
+    <t>2025-11-21</t>
+  </si>
+  <si>
+    <t>2025-11-22</t>
+  </si>
+  <si>
     <t>Reason</t>
   </si>
   <si>
@@ -305,13 +311,13 @@
     <t>Passed</t>
   </si>
   <si>
+    <t>Duplicate, Google chose different canonical than user</t>
+  </si>
+  <si>
+    <t>Google systems</t>
+  </si>
+  <si>
     <t>Crawled - currently not indexed</t>
-  </si>
-  <si>
-    <t>Google systems</t>
-  </si>
-  <si>
-    <t>Duplicate, Google chose different canonical than user</t>
   </si>
   <si>
     <t>Discovered - currently not indexed</t>
@@ -379,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -417,28 +423,28 @@
       <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>23.0</v>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>5</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B4" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>23.0</v>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>5</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="5">
@@ -452,7 +458,7 @@
         <v>23.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="6">
@@ -466,7 +472,7 @@
         <v>23.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -480,7 +486,7 @@
         <v>23.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="8">
@@ -494,7 +500,7 @@
         <v>23.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
@@ -502,13 +508,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>4.0</v>
+        <v>11.0</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>23.0</v>
+        <v>38.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>7.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="10">
@@ -516,13 +522,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>4.0</v>
+        <v>11.0</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>23.0</v>
+        <v>38.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="11">
@@ -536,7 +542,7 @@
         <v>38.0</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>17.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +556,7 @@
         <v>38.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="13">
@@ -558,13 +564,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
         <v>38.0</v>
-      </c>
-      <c r="D13" t="n" s="0">
-        <v>11.0</v>
       </c>
     </row>
     <row r="14">
@@ -572,13 +578,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="n" s="0">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>38.0</v>
+        <v>45.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>18.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="15">
@@ -592,7 +598,7 @@
         <v>45.0</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>38.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="16">
@@ -603,10 +609,10 @@
         <v>4.0</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>45.0</v>
+        <v>55.0</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>46.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="17">
@@ -617,10 +623,10 @@
         <v>4.0</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>45.0</v>
+        <v>55.0</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +640,7 @@
         <v>55.0</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>23.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="19">
@@ -648,7 +654,7 @@
         <v>55.0</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>33.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="20">
@@ -656,13 +662,13 @@
         <v>23</v>
       </c>
       <c r="B20" t="n" s="0">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>55.0</v>
+        <v>60.0</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>41.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="21">
@@ -670,13 +676,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="n" s="0">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="C21" t="n" s="0">
-        <v>55.0</v>
+        <v>60.0</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>46.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="22">
@@ -690,7 +696,7 @@
         <v>60.0</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>44.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="23">
@@ -698,13 +704,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="n" s="0">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="C23" t="n" s="0">
-        <v>60.0</v>
+        <v>76.0</v>
       </c>
       <c r="D23" t="n" s="0">
-        <v>33.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="24">
@@ -712,13 +718,13 @@
         <v>27</v>
       </c>
       <c r="B24" t="n" s="0">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="C24" t="n" s="0">
-        <v>60.0</v>
+        <v>76.0</v>
       </c>
       <c r="D24" t="n" s="0">
-        <v>35.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="25">
@@ -732,7 +738,7 @@
         <v>76.0</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>38.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="26">
@@ -746,7 +752,7 @@
         <v>76.0</v>
       </c>
       <c r="D26" t="n" s="0">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="27">
@@ -754,13 +760,13 @@
         <v>30</v>
       </c>
       <c r="B27" t="n" s="0">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="C27" t="n" s="0">
-        <v>76.0</v>
+        <v>88.0</v>
       </c>
       <c r="D27" t="n" s="0">
-        <v>40.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="28">
@@ -768,13 +774,13 @@
         <v>31</v>
       </c>
       <c r="B28" t="n" s="0">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="C28" t="n" s="0">
-        <v>76.0</v>
+        <v>88.0</v>
       </c>
       <c r="D28" t="n" s="0">
-        <v>43.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="29">
@@ -788,7 +794,7 @@
         <v>88.0</v>
       </c>
       <c r="D29" t="n" s="0">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="30">
@@ -796,13 +802,13 @@
         <v>33</v>
       </c>
       <c r="B30" t="n" s="0">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="C30" t="n" s="0">
-        <v>88.0</v>
+        <v>119.0</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>41.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="31">
@@ -810,13 +816,13 @@
         <v>34</v>
       </c>
       <c r="B31" t="n" s="0">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="C31" t="n" s="0">
-        <v>88.0</v>
+        <v>119.0</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>30.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="32">
@@ -830,7 +836,7 @@
         <v>119.0</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>52.0</v>
+        <v>87.0</v>
       </c>
     </row>
     <row r="33">
@@ -844,7 +850,7 @@
         <v>119.0</v>
       </c>
       <c r="D33" t="n" s="0">
-        <v>61.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="34">
@@ -852,13 +858,13 @@
         <v>37</v>
       </c>
       <c r="B34" t="n" s="0">
-        <v>8.0</v>
+        <v>147.0</v>
       </c>
       <c r="C34" t="n" s="0">
-        <v>119.0</v>
+        <v>130.0</v>
       </c>
       <c r="D34" t="n" s="0">
-        <v>87.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="35">
@@ -866,13 +872,13 @@
         <v>38</v>
       </c>
       <c r="B35" t="n" s="0">
-        <v>8.0</v>
+        <v>147.0</v>
       </c>
       <c r="C35" t="n" s="0">
-        <v>119.0</v>
+        <v>130.0</v>
       </c>
       <c r="D35" t="n" s="0">
-        <v>104.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="36">
@@ -886,7 +892,7 @@
         <v>130.0</v>
       </c>
       <c r="D36" t="n" s="0">
-        <v>77.0</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="37">
@@ -894,7 +900,7 @@
         <v>40</v>
       </c>
       <c r="B37" t="n" s="0">
-        <v>147.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" t="n" s="0">
         <v>130.0</v>
@@ -908,13 +914,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="n" s="0">
-        <v>147.0</v>
+        <v>4.0</v>
       </c>
       <c r="C38" t="n" s="0">
         <v>130.0</v>
       </c>
       <c r="D38" t="n" s="0">
-        <v>83.0</v>
+        <v>85.0</v>
       </c>
     </row>
     <row r="39">
@@ -928,7 +934,7 @@
         <v>130.0</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>67.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="40">
@@ -942,7 +948,7 @@
         <v>130.0</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>85.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="41">
@@ -950,13 +956,13 @@
         <v>44</v>
       </c>
       <c r="B41" t="n" s="0">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C41" t="n" s="0">
-        <v>130.0</v>
+        <v>128.0</v>
       </c>
       <c r="D41" t="n" s="0">
-        <v>48.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="42">
@@ -964,13 +970,13 @@
         <v>45</v>
       </c>
       <c r="B42" t="n" s="0">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C42" t="n" s="0">
-        <v>130.0</v>
+        <v>128.0</v>
       </c>
       <c r="D42" t="n" s="0">
-        <v>52.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="43">
@@ -984,7 +990,7 @@
         <v>128.0</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>61.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="44">
@@ -992,13 +998,13 @@
         <v>47</v>
       </c>
       <c r="B44" t="n" s="0">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C44" t="n" s="0">
-        <v>128.0</v>
+        <v>127.0</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>54.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="45">
@@ -1006,13 +1012,13 @@
         <v>48</v>
       </c>
       <c r="B45" t="n" s="0">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C45" t="n" s="0">
-        <v>128.0</v>
+        <v>127.0</v>
       </c>
       <c r="D45" t="n" s="0">
-        <v>45.0</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="46">
@@ -1026,7 +1032,7 @@
         <v>127.0</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>46.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1046,7 @@
         <v>127.0</v>
       </c>
       <c r="D47" t="n" s="0">
-        <v>74.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="48">
@@ -1048,13 +1054,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="n" s="0">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C48" t="n" s="0">
-        <v>127.0</v>
+        <v>126.0</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>60.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="49">
@@ -1062,13 +1068,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="n" s="0">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C49" t="n" s="0">
-        <v>127.0</v>
+        <v>126.0</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>61.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="50">
@@ -1082,7 +1088,7 @@
         <v>126.0</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>54.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="51">
@@ -1090,13 +1096,13 @@
         <v>54</v>
       </c>
       <c r="B51" t="n" s="0">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
       <c r="C51" t="n" s="0">
-        <v>126.0</v>
+        <v>121.0</v>
       </c>
       <c r="D51" t="n" s="0">
-        <v>51.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="52">
@@ -1104,13 +1110,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="n" s="0">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
       <c r="C52" t="n" s="0">
-        <v>126.0</v>
+        <v>121.0</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>36.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="53">
@@ -1124,7 +1130,7 @@
         <v>121.0</v>
       </c>
       <c r="D53" t="n" s="0">
-        <v>55.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="54">
@@ -1138,7 +1144,7 @@
         <v>121.0</v>
       </c>
       <c r="D54" t="n" s="0">
-        <v>41.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="55">
@@ -1146,13 +1152,13 @@
         <v>58</v>
       </c>
       <c r="B55" t="n" s="0">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="C55" t="n" s="0">
-        <v>121.0</v>
+        <v>115.0</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>56.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="56">
@@ -1160,13 +1166,13 @@
         <v>59</v>
       </c>
       <c r="B56" t="n" s="0">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="C56" t="n" s="0">
-        <v>121.0</v>
+        <v>115.0</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>15.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="57">
@@ -1180,7 +1186,7 @@
         <v>115.0</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="58">
@@ -1188,13 +1194,13 @@
         <v>61</v>
       </c>
       <c r="B58" t="n" s="0">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C58" t="n" s="0">
-        <v>115.0</v>
+        <v>114.0</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="59">
@@ -1202,13 +1208,13 @@
         <v>62</v>
       </c>
       <c r="B59" t="n" s="0">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C59" t="n" s="0">
-        <v>115.0</v>
+        <v>114.0</v>
       </c>
       <c r="D59" t="n" s="0">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="60">
@@ -1222,7 +1228,7 @@
         <v>114.0</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="61">
@@ -1236,7 +1242,7 @@
         <v>114.0</v>
       </c>
       <c r="D61" t="n" s="0">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="62">
@@ -1244,13 +1250,13 @@
         <v>65</v>
       </c>
       <c r="B62" t="n" s="0">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
       <c r="C62" t="n" s="0">
-        <v>114.0</v>
+        <v>107.0</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>30.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="63">
@@ -1258,13 +1264,13 @@
         <v>66</v>
       </c>
       <c r="B63" t="n" s="0">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
       <c r="C63" t="n" s="0">
-        <v>114.0</v>
+        <v>107.0</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>23.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="64">
@@ -1278,7 +1284,7 @@
         <v>107.0</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="65">
@@ -1286,13 +1292,13 @@
         <v>68</v>
       </c>
       <c r="B65" t="n" s="0">
-        <v>28.0</v>
+        <v>36.0</v>
       </c>
       <c r="C65" t="n" s="0">
-        <v>107.0</v>
+        <v>99.0</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>27.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="66">
@@ -1300,13 +1306,13 @@
         <v>69</v>
       </c>
       <c r="B66" t="n" s="0">
-        <v>28.0</v>
+        <v>36.0</v>
       </c>
       <c r="C66" t="n" s="0">
-        <v>107.0</v>
+        <v>99.0</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>28.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="67">
@@ -1320,7 +1326,7 @@
         <v>99.0</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="68">
@@ -1334,7 +1340,7 @@
         <v>99.0</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>19.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="69">
@@ -1348,7 +1354,7 @@
         <v>99.0</v>
       </c>
       <c r="D69" t="n" s="0">
-        <v>9.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="70">
@@ -1362,7 +1368,7 @@
         <v>99.0</v>
       </c>
       <c r="D70" t="n" s="0">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="71">
@@ -1376,7 +1382,7 @@
         <v>99.0</v>
       </c>
       <c r="D71" t="n" s="0">
-        <v>15.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="72">
@@ -1384,13 +1390,13 @@
         <v>75</v>
       </c>
       <c r="B72" t="n" s="0">
-        <v>36.0</v>
+        <v>38.0</v>
       </c>
       <c r="C72" t="n" s="0">
-        <v>99.0</v>
+        <v>97.0</v>
       </c>
       <c r="D72" t="n" s="0">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="73">
@@ -1398,13 +1404,13 @@
         <v>76</v>
       </c>
       <c r="B73" t="n" s="0">
-        <v>36.0</v>
+        <v>38.0</v>
       </c>
       <c r="C73" t="n" s="0">
-        <v>99.0</v>
+        <v>97.0</v>
       </c>
       <c r="D73" t="n" s="0">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="74">
@@ -1418,7 +1424,7 @@
         <v>97.0</v>
       </c>
       <c r="D74" t="n" s="0">
-        <v>16.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="75">
@@ -1432,7 +1438,7 @@
         <v>97.0</v>
       </c>
       <c r="D75" t="n" s="0">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="76">
@@ -1440,13 +1446,13 @@
         <v>79</v>
       </c>
       <c r="B76" t="n" s="0">
-        <v>38.0</v>
+        <v>43.0</v>
       </c>
       <c r="C76" t="n" s="0">
-        <v>97.0</v>
+        <v>92.0</v>
       </c>
       <c r="D76" t="n" s="0">
-        <v>10.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="77">
@@ -1454,13 +1460,13 @@
         <v>80</v>
       </c>
       <c r="B77" t="n" s="0">
-        <v>38.0</v>
+        <v>43.0</v>
       </c>
       <c r="C77" t="n" s="0">
-        <v>97.0</v>
+        <v>92.0</v>
       </c>
       <c r="D77" t="n" s="0">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="78">
@@ -1474,7 +1480,7 @@
         <v>92.0</v>
       </c>
       <c r="D78" t="n" s="0">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="79">
@@ -1482,13 +1488,13 @@
         <v>82</v>
       </c>
       <c r="B79" t="n" s="0">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
       <c r="C79" t="n" s="0">
-        <v>92.0</v>
+        <v>89.0</v>
       </c>
       <c r="D79" t="n" s="0">
-        <v>16.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="80">
@@ -1496,13 +1502,41 @@
         <v>83</v>
       </c>
       <c r="B80" t="n" s="0">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
       <c r="C80" t="n" s="0">
-        <v>92.0</v>
+        <v>89.0</v>
       </c>
       <c r="D80" t="n" s="0">
-        <v>20.0</v>
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B81" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="C81" t="n" s="0">
+        <v>89.0</v>
+      </c>
+      <c r="D81" t="n" s="0">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B82" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="C82" t="n" s="0">
+        <v>89.0</v>
+      </c>
+      <c r="D82" t="n" s="0">
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
@@ -1520,27 +1554,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
@@ -1548,27 +1582,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>89</v>
-      </c>
       <c r="C3" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>1.0</v>
@@ -1576,13 +1610,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>0.0</v>
@@ -1590,27 +1624,27 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>95</v>
-      </c>
       <c r="D6" t="n" s="0">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>97</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>95</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>6.0</v>
@@ -1618,13 +1652,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>97</v>
-      </c>
       <c r="C8" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>0.0</v>
@@ -1645,16 +1679,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1672,18 +1706,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>